<commit_message>
enemy AI being programmed
enemy AI being programmed
captain spheres being added to control armies
report writing
game testing
</commit_message>
<xml_diff>
--- a/documentation/loops and systemm plans.xlsx
+++ b/documentation/loops and systemm plans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\3RD YEAR\COMP3000\github repo\Defend-Capture\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84BB2929-0392-4BA8-AC72-7807CC51C194}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0937FD12-09FC-474B-BABC-39A51A8CBD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3D41F141-337B-4EA4-A077-7D08A8DBCF55}"/>
+    <workbookView xWindow="38280" yWindow="1965" windowWidth="29040" windowHeight="15840" xr2:uid="{3D41F141-337B-4EA4-A077-7D08A8DBCF55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>no reactor</t>
   </si>
@@ -117,7 +117,16 @@
     <t>Vehicles &gt; soidlers</t>
   </si>
   <si>
-    <t xml:space="preserve">Rocker Paper Scissors System </t>
+    <t xml:space="preserve">Rock Paper Scissors System </t>
+  </si>
+  <si>
+    <t>Reactor</t>
+  </si>
+  <si>
+    <t>supplies power to base, allows use of lvl 1 buildings</t>
+  </si>
+  <si>
+    <t>allows use of lvl 2 upgrades</t>
   </si>
 </sst>
 </file>
@@ -133,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,18 +199,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -205,6 +211,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +538,7 @@
   <dimension ref="B4:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,11 +551,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
       <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
@@ -558,11 +573,11 @@
       <c r="H5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -575,11 +590,11 @@
       <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
@@ -590,11 +605,11 @@
       <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -602,12 +617,12 @@
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>5</v>
@@ -615,83 +630,89 @@
       <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+    <row r="16" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>